<commit_message>
BAJAJ-PL MIS Base Page...
</commit_message>
<xml_diff>
--- a/media/FULLERTON_RECOVERY/Billing/PAYOUT_FULLERTON_RECOVERY.xlsx
+++ b/media/FULLERTON_RECOVERY/Billing/PAYOUT_FULLERTON_RECOVERY.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,22 +497,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>14135912.48</v>
+        <v>9170193.810000001</v>
       </c>
       <c r="D2" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E2" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2" t="n">
-        <v>386172</v>
+        <v>161172</v>
       </c>
       <c r="H2" t="n">
-        <v>2.73</v>
+        <v>1.76</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>61787.52</v>
+        <v>25787.52</v>
       </c>
     </row>
     <row r="3">
@@ -535,22 +535,22 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>11688940.48</v>
+        <v>17749604.12</v>
       </c>
       <c r="D3" t="n">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E3" t="n">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="F3" t="n">
         <v>5</v>
       </c>
       <c r="G3" t="n">
-        <v>131095</v>
+        <v>181585</v>
       </c>
       <c r="H3" t="n">
-        <v>1.12</v>
+        <v>1.02</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -558,7 +558,7 @@
         </is>
       </c>
       <c r="J3" t="n">
-        <v>22941.625</v>
+        <v>31777.375</v>
       </c>
     </row>
     <row r="4">
@@ -573,30 +573,30 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3152808.36</v>
+        <v>1448782.22</v>
       </c>
       <c r="D4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>135000</v>
+        <v>5000</v>
       </c>
       <c r="H4" t="n">
-        <v>4.28</v>
+        <v>0.35</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>22.5%</t>
+          <t>20%</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>30375</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5">
@@ -611,22 +611,22 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7452298.92</v>
+        <v>10197523.39</v>
       </c>
       <c r="D5" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E5" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5" t="n">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="H5" t="n">
-        <v>0.27</v>
+        <v>0.29</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>4500</v>
+        <v>6750</v>
       </c>
     </row>
     <row r="6">
@@ -649,22 +649,22 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6208060.53</v>
+        <v>13244323.61</v>
       </c>
       <c r="D6" t="n">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="E6" t="n">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>110000</v>
+        <v>15000</v>
       </c>
       <c r="H6" t="n">
-        <v>1.77</v>
+        <v>0.11</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>27500</v>
+        <v>3750</v>
       </c>
     </row>
     <row r="7">
@@ -687,30 +687,30 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1040835.41</v>
+        <v>1828497.2</v>
       </c>
       <c r="D7" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E7" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1.37</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>32.5%</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>0</v>
+        <v>8125</v>
       </c>
     </row>
     <row r="8">
@@ -725,22 +725,22 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1668156.97</v>
+        <v>2805254.55</v>
       </c>
       <c r="D8" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -748,7 +748,7 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>2400</v>
       </c>
     </row>
     <row r="9">
@@ -763,13 +763,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>8744105.789999999</v>
+        <v>7479921.47</v>
       </c>
       <c r="D9" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F9" t="n">
         <v>2</v>
@@ -778,7 +778,7 @@
         <v>30000</v>
       </c>
       <c r="H9" t="n">
-        <v>0.34</v>
+        <v>0.4</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -797,17 +797,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>V4</t>
+          <t>V3</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2276181.96</v>
+        <v>550961.3100000001</v>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -820,7 +820,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>22.5%</t>
+          <t>20%</t>
         </is>
       </c>
       <c r="J10" t="n">
@@ -835,34 +835,34 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>V5</t>
+          <t>V4</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2345202.44</v>
+        <v>4588615.25</v>
       </c>
       <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="n">
         <v>8</v>
-      </c>
-      <c r="E11" t="n">
-        <v>7</v>
       </c>
       <c r="F11" t="n">
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>19000</v>
+        <v>10000</v>
       </c>
       <c r="H11" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.22</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>22.5%</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>4750</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="12">
@@ -873,17 +873,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>V6</t>
+          <t>V5</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1200787.62</v>
+        <v>4249598.26</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -896,11 +896,49 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>30%</t>
+          <t>25%</t>
         </is>
       </c>
       <c r="J12" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PL Self</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>V6</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1818015.45</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7</v>
+      </c>
+      <c r="E13" t="n">
+        <v>6</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>32000</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1.76</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>35%</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>11200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>